<commit_message>
fix lazy tab problem and fop access; closes #1041
</commit_message>
<xml_diff>
--- a/owlcms/src/main/resources/robi/RobiCategories.xlsx
+++ b/owlcms/src/main/resources/robi/RobiCategories.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\agegroups\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamyj\git\owlcms4\owlcms\src\main\resources\robi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{56C709A1-8B92-43A8-A061-1D32E63A63E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2ED0D9EE-86C1-41C0-B99C-F0FAB1CD447A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3180" yWindow="1335" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BW Categories" sheetId="1" r:id="rId1"/>
@@ -221,18 +221,12 @@
       <name val="Arial"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF34A853"/>
-        <bgColor rgb="FF34A853"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -287,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -295,19 +289,16 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
@@ -530,7 +521,9 @@
   </sheetPr>
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2:F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
@@ -587,9 +580,7 @@
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="5">
-        <v>135</v>
-      </c>
+      <c r="F3" s="1"/>
       <c r="H3" s="3" t="s">
         <v>10</v>
       </c>
@@ -606,10 +597,8 @@
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="4">
-        <v>172</v>
-      </c>
-      <c r="H4" s="6" t="s">
+      <c r="F4" s="1"/>
+      <c r="H4" s="5" t="s">
         <v>12</v>
       </c>
     </row>
@@ -625,10 +614,8 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="4">
-        <v>221</v>
-      </c>
-      <c r="H5" s="7"/>
+      <c r="F5" s="1"/>
+      <c r="H5" s="6"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
@@ -641,15 +628,15 @@
         <v>55</v>
       </c>
       <c r="D6" s="4">
-        <v>294</v>
+        <v>265</v>
       </c>
       <c r="E6" s="4">
         <v>265</v>
       </c>
       <c r="F6" s="4">
-        <v>258</v>
-      </c>
-      <c r="H6" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>15</v>
       </c>
     </row>
@@ -664,13 +651,13 @@
         <v>61</v>
       </c>
       <c r="D7" s="4">
-        <v>318</v>
+        <v>307</v>
       </c>
       <c r="E7" s="4">
         <v>307</v>
       </c>
       <c r="F7" s="4">
-        <v>276</v>
+        <v>307</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -684,13 +671,13 @@
         <v>67</v>
       </c>
       <c r="D8" s="4">
-        <v>339</v>
+        <v>328</v>
       </c>
       <c r="E8" s="4">
         <v>328</v>
       </c>
       <c r="F8" s="4">
-        <v>306</v>
+        <v>328</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -704,13 +691,13 @@
         <v>73</v>
       </c>
       <c r="D9" s="4">
-        <v>364</v>
+        <v>351</v>
       </c>
       <c r="E9" s="4">
         <v>351</v>
       </c>
       <c r="F9" s="4">
-        <v>309</v>
+        <v>351</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,7 +711,7 @@
         <v>81</v>
       </c>
       <c r="D10" s="4">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E10" s="4">
         <v>374</v>
@@ -744,13 +731,13 @@
         <v>89</v>
       </c>
       <c r="D11" s="4">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E11" s="4">
         <v>395</v>
       </c>
       <c r="F11" s="4">
-        <v>357</v>
+        <v>395</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -764,13 +751,13 @@
         <v>96</v>
       </c>
       <c r="D12" s="4">
-        <v>416</v>
+        <v>397</v>
       </c>
       <c r="E12" s="4">
         <v>397</v>
       </c>
       <c r="F12" s="4">
-        <v>354</v>
+        <v>397</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -784,13 +771,13 @@
         <v>102</v>
       </c>
       <c r="D13" s="4">
-        <v>412</v>
+        <v>393</v>
       </c>
       <c r="E13" s="4">
         <v>393</v>
       </c>
       <c r="F13" s="4">
-        <v>386</v>
+        <v>393</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -804,12 +791,14 @@
         <v>109</v>
       </c>
       <c r="D14" s="4">
-        <v>435</v>
+        <v>417</v>
       </c>
       <c r="E14" s="4">
         <v>417</v>
       </c>
-      <c r="F14" s="1"/>
+      <c r="F14" s="4">
+        <v>417</v>
+      </c>
     </row>
     <row r="15" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
@@ -822,13 +811,13 @@
         <v>999</v>
       </c>
       <c r="D15" s="4">
-        <v>492</v>
+        <v>436</v>
       </c>
       <c r="E15" s="4">
         <v>436</v>
       </c>
       <c r="F15" s="4">
-        <v>396</v>
+        <v>436</v>
       </c>
       <c r="H15" s="1" t="s">
         <v>25</v>
@@ -860,9 +849,7 @@
       </c>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-      <c r="F17" s="4">
-        <v>135</v>
-      </c>
+      <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
@@ -875,13 +862,13 @@
         <v>45</v>
       </c>
       <c r="D18" s="4">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="E18" s="4">
         <v>179</v>
       </c>
       <c r="F18" s="4">
-        <v>172</v>
+        <v>179</v>
       </c>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -895,13 +882,13 @@
         <v>49</v>
       </c>
       <c r="D19" s="4">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="E19" s="4">
         <v>206</v>
       </c>
       <c r="F19" s="4">
-        <v>190</v>
+        <v>206</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -915,13 +902,13 @@
         <v>55</v>
       </c>
       <c r="D20" s="4">
-        <v>233</v>
+        <v>213</v>
       </c>
       <c r="E20" s="4">
         <v>213</v>
       </c>
       <c r="F20" s="4">
-        <v>198</v>
+        <v>213</v>
       </c>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -935,13 +922,13 @@
         <v>59</v>
       </c>
       <c r="D21" s="4">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="E21" s="4">
         <v>246</v>
       </c>
       <c r="F21" s="4">
-        <v>228</v>
+        <v>246</v>
       </c>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -954,14 +941,14 @@
       <c r="C22" s="4">
         <v>64</v>
       </c>
-      <c r="D22" s="4">
-        <v>261</v>
-      </c>
-      <c r="E22" s="8">
+      <c r="D22" s="7">
         <v>260</v>
       </c>
-      <c r="F22" s="4">
-        <v>233</v>
+      <c r="E22" s="7">
+        <v>260</v>
+      </c>
+      <c r="F22" s="7">
+        <v>260</v>
       </c>
     </row>
     <row r="23" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -974,14 +961,14 @@
       <c r="C23" s="4">
         <v>71</v>
       </c>
-      <c r="D23" s="4">
-        <v>273</v>
-      </c>
-      <c r="E23" s="8">
+      <c r="D23" s="7">
         <v>262</v>
       </c>
-      <c r="F23" s="4">
-        <v>230</v>
+      <c r="E23" s="7">
+        <v>262</v>
+      </c>
+      <c r="F23" s="7">
+        <v>262</v>
       </c>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -995,13 +982,13 @@
         <v>76</v>
       </c>
       <c r="D24" s="4">
-        <v>278</v>
+        <v>259</v>
       </c>
       <c r="E24" s="4">
         <v>259</v>
       </c>
       <c r="F24" s="4">
-        <v>229</v>
+        <v>259</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1015,13 +1002,13 @@
         <v>81</v>
       </c>
       <c r="D25" s="4">
-        <v>284</v>
+        <v>260</v>
       </c>
       <c r="E25" s="4">
         <v>260</v>
       </c>
-      <c r="F25" s="8">
-        <v>236</v>
+      <c r="F25" s="4">
+        <v>260</v>
       </c>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1035,12 +1022,14 @@
         <v>87</v>
       </c>
       <c r="D26" s="4">
-        <v>294</v>
+        <v>269</v>
       </c>
       <c r="E26" s="4">
         <v>269</v>
       </c>
-      <c r="F26" s="1"/>
+      <c r="F26" s="4">
+        <v>269</v>
+      </c>
     </row>
     <row r="27" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
@@ -1053,13 +1042,13 @@
         <v>999</v>
       </c>
       <c r="D27" s="4">
-        <v>335</v>
+        <v>332</v>
       </c>
       <c r="E27" s="4">
         <v>332</v>
       </c>
       <c r="F27" s="4">
-        <v>255</v>
+        <v>332</v>
       </c>
       <c r="H27" s="1" t="s">
         <v>39</v>
@@ -2087,22 +2076,22 @@
       <c r="G1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="H1" s="11" t="s">
+      <c r="H1" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="12"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="8"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="8"/>
+      <c r="P1" s="8"/>
+      <c r="Q1" s="8"/>
+      <c r="R1" s="8"/>
+      <c r="S1" s="8"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
     </row>
     <row r="2" spans="1:22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2121,7 +2110,7 @@
       <c r="F2" s="4">
         <v>999</v>
       </c>
-      <c r="G2" s="10" t="b">
+      <c r="G2" s="9" t="b">
         <v>1</v>
       </c>
       <c r="H2" s="1" t="s">
@@ -2183,7 +2172,7 @@
       <c r="F3" s="4">
         <v>999</v>
       </c>
-      <c r="G3" s="10" t="b">
+      <c r="G3" s="9" t="b">
         <v>1</v>
       </c>
       <c r="H3" s="1"/>

</xml_diff>